<commit_message>
préparation publication 4.0.2 71af116d2ff222748d4b1c375e1fee643722675b
</commit_message>
<xml_diff>
--- a/Publication-402/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/Publication-402/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.2-ballot-3</t>
+    <t>4.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-19T08:36:41+00:00</t>
+    <t>2024-06-19T09:38:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>